<commit_message>
Correction tre r394 0e2804a9eb243d0906a20d4743528ab80298e7b7
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/ValueSet-competenceMetier-vs.xlsx
+++ b/poc-professionnel/ig/ValueSet-competenceMetier-vs.xlsx
@@ -37,7 +37,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>CompetencemetierVs</t>
+    <t>CompetencemetiereVs</t>
   </si>
   <si>
     <t>Title</t>
@@ -55,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-21T14:08:48+00:00</t>
+    <t>2025-07-22T15:23:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -103,10 +103,10 @@
     <t>System URI</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/terminologies/CodeSystem-TRE-R394-competence-metier</t>
-  </si>
-  <si>
     <t>https://interop.esante.gouv.fr/terminologies/CodeSystem-TRE-R01-EnsembleSavoirFaire-CISIS</t>
+  </si>
+  <si>
+    <t>https://smt.esante.gouv.fr/fhir/CodeSystem/tre-r394-competence-metier</t>
   </si>
 </sst>
 </file>

</xml_diff>